<commit_message>
All SSE labs finished
</commit_message>
<xml_diff>
--- a/Radiotechnics_Labs/6_sem/Lab05/data.xlsx
+++ b/Radiotechnics_Labs/6_sem/Lab05/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nekha\OneDrive\GitHub\Labs\Radiotechnics_Labs\6_sem\Lab05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{42F17FC6-771D-435E-9C01-9C1ED4E98DA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{E347C38C-6AE3-4997-BBC6-5F47CA9A1B31}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{42F17FC6-771D-435E-9C01-9C1ED4E98DA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{74EC048D-E762-453A-B6A2-C5991E684554}"/>
   <bookViews>
-    <workbookView xWindow="16628" yWindow="7403" windowWidth="18225" windowHeight="11422" xr2:uid="{36EF286A-0632-4BBD-BA19-79249F406910}"/>
+    <workbookView xWindow="3832" yWindow="1425" windowWidth="18225" windowHeight="11423" activeTab="1" xr2:uid="{36EF286A-0632-4BBD-BA19-79249F406910}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Частота:</t>
   </si>
@@ -61,6 +62,54 @@
   </si>
   <si>
     <t>Усиление необходимое для генерации</t>
+  </si>
+  <si>
+    <t>Коэффициент обратной связи</t>
+  </si>
+  <si>
+    <t>370 мВ</t>
+  </si>
+  <si>
+    <t>110 мВ</t>
+  </si>
+  <si>
+    <t>K_VT2</t>
+  </si>
+  <si>
+    <t>K_VT1</t>
+  </si>
+  <si>
+    <t>Частотомер</t>
+  </si>
+  <si>
+    <t>Коэффициент передачи при стандарных</t>
+  </si>
+  <si>
+    <t>Ku</t>
+  </si>
+  <si>
+    <t>Vп, В</t>
+  </si>
+  <si>
+    <t>Vамплитуды, мВ</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Уход частоты</t>
+  </si>
+  <si>
+    <t>кГц</t>
+  </si>
+  <si>
+    <t>Гц</t>
   </si>
 </sst>
 </file>
@@ -416,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61848B87-72DC-4174-9A39-41801A053835}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -506,4 +555,330 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4855CA0A-F2D9-4EC1-8F54-7D07114AC54D}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="15.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <v>1.35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <v>1.3460000000000001</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <v>1.006</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>1.337</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <v>1.335</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>1.3320000000000001</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>734</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>530</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B26">
+        <v>1.0004999999999999</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B27">
+        <v>1.00068</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B28">
+        <v>989.8</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B29">
+        <v>989.6</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <v>971.7</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31">
+        <v>180</v>
+      </c>
+      <c r="D31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>